<commit_message>
ic stock2 ,octopart email
</commit_message>
<xml_diff>
--- a/Tender/Task.xlsx
+++ b/Tender/Task.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhe/PycharmProjects/TransitTech/Tender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhe/PycharmProjects/YJCX_AI/Tender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46C9ED1-1E3C-8045-91B6-276DCB4A4D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64437B7A-8CB8-A446-93CC-28DAEC7E7ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44560" yWindow="1580" windowWidth="39160" windowHeight="17580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5240" yWindow="8340" windowWidth="30240" windowHeight="17760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="tender" sheetId="2" r:id="rId2"/>
     <sheet name="b2b-center2" sheetId="3" r:id="rId3"/>
+    <sheet name="ros" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8010" uniqueCount="4331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8240" uniqueCount="4424">
   <si>
     <t>No</t>
   </si>
@@ -13015,13 +13016,366 @@
   </si>
   <si>
     <t>0,41 руб. (сумма, НДС не облагается)</t>
+  </si>
+  <si>
+    <t>SIEMENS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electromechanical &amp; Automation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCHNEIDER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Danfoss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUNON</t>
+  </si>
+  <si>
+    <t>Lenze</t>
+  </si>
+  <si>
+    <t>MOXA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EATON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复合型品牌，部分产品超出业务范围</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kollmorgen</t>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lafert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yaskawa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semiconductor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRACO POWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Supply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XP POWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELTA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEANWELL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Supply &amp; Semiconductor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MORNSUN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VICOR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PHOENIX</t>
+  </si>
+  <si>
+    <t>Connectors &amp; Power supply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEIPU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connectors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEGSON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMPHENOL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TE CONNECTIVITY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KLS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONNFLY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WEIDMULLER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t>HARTING</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>PANASONIC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MITSUBISHI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICRON</t>
+  </si>
+  <si>
+    <t>SEMIKRON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ANALOG DEVICES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEXAS INSTRUMENTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SENSATA</t>
+  </si>
+  <si>
+    <t>HAMAMATSU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scientific Instrument</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IFM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIMTEC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">AVAGO </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BROADCOM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPCOS</t>
+  </si>
+  <si>
+    <t>FUJI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HONEYWELL</t>
+  </si>
+  <si>
+    <t>HUBER+SUHNER</t>
+  </si>
+  <si>
+    <t>INFINEON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>International Rectifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IXYS</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LATTICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICROCHIP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MICROSEMI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MURATA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NEXPERIA</t>
+  </si>
+  <si>
+    <t>NXP</t>
+  </si>
+  <si>
+    <t>RENESAS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEMTECH</t>
+  </si>
+  <si>
+    <t>SILICON LABS</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VISHAY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XILINX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YAGEO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>транзистор</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IGBT</t>
+  </si>
+  <si>
+    <t>мультиплексор</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">радиокомпонентов </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DRAM</t>
+  </si>
+  <si>
+    <t>Rectifier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>выпрямитель</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>резистор</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>датчик</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRAM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>электронных компонентов</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Газпром</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ИРЗ ТЭК</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>integrated chips</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Новатек-Электро (Санкт-Петербург)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>АО "ИРЗ"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ПРОМЫШЛЕННЫЕ ИННОВАЦИИ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13079,6 +13433,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -13094,7 +13456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -13102,12 +13464,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -13115,6 +13492,24 @@
     <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -13762,7 +14157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I888"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A861" workbookViewId="0"/>
+    <sheetView topLeftCell="A861" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
@@ -39525,4 +39920,880 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FC2443-C583-8146-BC18-747A34831A69}">
+  <dimension ref="A1:D82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection sqref="A1:A82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>4331</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4334</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4335</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4336</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7" t="s">
+        <v>4337</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="7" t="s">
+        <v>4339</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="7" t="s">
+        <v>4340</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4333</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="7" t="s">
+        <v>4342</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="7" t="s">
+        <v>4344</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4345</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4332</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4347</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4349</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4351</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>4333</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="7" t="s">
+        <v>4352</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="7" t="s">
+        <v>4353</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4354</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7" t="s">
+        <v>4355</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7" t="s">
+        <v>4356</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4348</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="7" t="s">
+        <v>4357</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>4358</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="7" t="s">
+        <v>4359</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="7" t="s">
+        <v>4361</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="7" t="s">
+        <v>4362</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="7" t="s">
+        <v>4363</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="7" t="s">
+        <v>4364</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7" t="s">
+        <v>4365</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="8" t="s">
+        <v>4366</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="7" t="s">
+        <v>4367</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="7" t="s">
+        <v>4368</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="7" t="s">
+        <v>4369</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7" t="s">
+        <v>4370</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>4360</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>4371</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>4333</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>4372</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>4333</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="7" t="s">
+        <v>4373</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="7" t="s">
+        <v>4374</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="7" t="s">
+        <v>4375</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="7" t="s">
+        <v>4376</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="7" t="s">
+        <v>4377</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="9" t="s">
+        <v>4378</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="7" t="s">
+        <v>4379</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>4380</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="7" t="s">
+        <v>4381</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="7" t="s">
+        <v>4382</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="7" t="s">
+        <v>4383</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="7" t="s">
+        <v>4384</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="7" t="s">
+        <v>4385</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="7" t="s">
+        <v>4386</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="7" t="s">
+        <v>4387</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="7" t="s">
+        <v>4388</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="7" t="s">
+        <v>4389</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="7" t="s">
+        <v>4390</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="7" t="s">
+        <v>4391</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="7" t="s">
+        <v>4392</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="7" t="s">
+        <v>4393</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="7" t="s">
+        <v>4394</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="7" t="s">
+        <v>4395</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="7" t="s">
+        <v>4396</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="7" t="s">
+        <v>4397</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="7" t="s">
+        <v>4398</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="7" t="s">
+        <v>4399</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="7" t="s">
+        <v>4400</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="7" t="s">
+        <v>4401</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="7" t="s">
+        <v>4402</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>4403</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>4404</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>4405</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4346</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="7" t="s">
+        <v>4407</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>4408</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>4409</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="7" t="s">
+        <v>4410</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>4411</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>4412</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>4413</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>4414</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>4415</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>4416</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>4417</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>4406</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15">
+      <c r="A79" s="10" t="s">
+        <v>4419</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="45">
+      <c r="A80" s="11" t="s">
+        <v>4421</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>4422</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="30">
+      <c r="A82" s="10" t="s">
+        <v>4423</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4420</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>